<commit_message>
added continents to town model
</commit_message>
<xml_diff>
--- a/travels/db/badges.xlsx
+++ b/travels/db/badges.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kathrin/development/project-4/travels/db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA49E8CE-862A-7842-9CA8-E915DC8D6722}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24119C2A-DD8E-B64A-99D8-D311DFAD011F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25460" windowHeight="15000" xr2:uid="{B9AD43F2-C69D-5247-901B-E34DC6958E20}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="415">
   <si>
     <t>Japan</t>
   </si>
@@ -2923,6 +2923,9 @@
       </rPr>
       <t>https://restcountries.eu/data/zwe.svg</t>
     </r>
+  </si>
+  <si>
+    <t>Oceania</t>
   </si>
 </sst>
 </file>
@@ -3290,8 +3293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19E1AC67-419D-4746-879D-BEFE92ACFE5A}">
   <dimension ref="A1:C217"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A191" workbookViewId="0">
+      <selection activeCell="A208" sqref="A208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5771,11 +5774,11 @@
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>33</v>
+        <v>414</v>
       </c>
       <c r="B207" t="str">
         <f t="shared" si="4"/>
-        <v>Visit at least one country on the continent of Australia</v>
+        <v>Visit at least one country on the continent of Oceania</v>
       </c>
       <c r="C207" t="s">
         <v>229</v>

</xml_diff>